<commit_message>
basic version of monte carlo simulation
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet state="visible" name="HW Architecture" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="Availability" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="newSheet" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
   <si>
     <t>from</t>
   </si>
@@ -159,13 +160,52 @@
   </si>
   <si>
     <t>ControllerBox</t>
+  </si>
+  <si>
+    <t>PBSSD</t>
+  </si>
+  <si>
+    <t>MTBF</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
+    <t>DIMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIC </t>
+  </si>
+  <si>
+    <t>SSD</t>
+  </si>
+  <si>
+    <t>BP</t>
+  </si>
+  <si>
+    <t>Riser card</t>
+  </si>
+  <si>
+    <t>Fan</t>
+  </si>
+  <si>
+    <t>AOM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSU </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -198,8 +238,13 @@
       <color rgb="FF000000"/>
       <name val="&quot;Malgun Gothic&quot;"/>
     </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="&quot;Malgun Gothic&quot;"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,8 +257,14 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border/>
     <border>
       <left style="thin">
@@ -259,11 +310,30 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -301,6 +371,14 @@
     <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
+    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="6" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -314,6 +392,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -2146,14 +2228,14 @@
         <v>41</v>
       </c>
       <c r="C7" s="14">
-        <v>4194389.0</v>
+        <v>2500000.0</v>
       </c>
       <c r="D7" s="14">
         <v>8.0</v>
       </c>
       <c r="E7" s="9">
         <f t="shared" si="1"/>
-        <v>0.9999980927</v>
+        <v>0.9999968</v>
       </c>
       <c r="F7" s="11">
         <v>3.0</v>
@@ -3197,4 +3279,107 @@
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="4">
+      <c r="A4" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="18">
+        <v>367985.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3.51E8</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="18">
+        <v>3472222.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="18">
+        <v>4194389.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="18">
+        <v>2500000.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" s="18">
+        <v>9247903.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="18">
+        <v>1.3764075E7</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="18">
+        <v>1500000.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="18">
+        <v>8249472.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="18">
+        <v>241296.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fix bug and add simulation
</commit_message>
<xml_diff>
--- a/availability.xlsx
+++ b/availability.xlsx
@@ -1,19 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\주우스\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30E761C6-EA14-470F-A1AA-88F37300BE6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="HW Architecture" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Availability" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="newSheet" sheetId="3" r:id="rId6"/>
+    <sheet name="HW Architecture" sheetId="1" r:id="rId1"/>
+    <sheet name="Availability" sheetId="2" r:id="rId2"/>
+    <sheet name="newSheet" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="139">
   <si>
     <t>from</t>
   </si>
@@ -42,48 +64,12 @@
     <t>NVMeEnclosure0</t>
   </si>
   <si>
-    <t>pci0</t>
-  </si>
-  <si>
-    <t>pci1</t>
-  </si>
-  <si>
-    <t>dfm0</t>
-  </si>
-  <si>
-    <t>dfm1</t>
-  </si>
-  <si>
-    <t>dfm2</t>
-  </si>
-  <si>
-    <t>dfm3</t>
-  </si>
-  <si>
     <t>host_module1</t>
   </si>
   <si>
     <t>NVMeEnclosure1</t>
   </si>
   <si>
-    <t>pci2</t>
-  </si>
-  <si>
-    <t>pci3</t>
-  </si>
-  <si>
-    <t>dfm4</t>
-  </si>
-  <si>
-    <t>dfm5</t>
-  </si>
-  <si>
-    <t>dfm6</t>
-  </si>
-  <si>
-    <t>dfm7</t>
-  </si>
-  <si>
     <t>switch1</t>
   </si>
   <si>
@@ -117,9 +103,6 @@
     <t>8G</t>
   </si>
   <si>
-    <t>Redundancy</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -135,12 +118,6 @@
     <t>backend_module</t>
   </si>
   <si>
-    <t>pci</t>
-  </si>
-  <si>
-    <t>dfm</t>
-  </si>
-  <si>
     <t>module</t>
   </si>
   <si>
@@ -156,9 +133,6 @@
     <t>NVMeEnclosure</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>ControllerBox</t>
   </si>
   <si>
@@ -196,52 +170,727 @@
   </si>
   <si>
     <t xml:space="preserve">PSU </t>
+  </si>
+  <si>
+    <t>ssd0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd2</t>
+  </si>
+  <si>
+    <t>ssd2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd3</t>
+  </si>
+  <si>
+    <t>ssd3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd4</t>
+  </si>
+  <si>
+    <t>ssd4</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd5</t>
+  </si>
+  <si>
+    <t>ssd6</t>
+  </si>
+  <si>
+    <t>ssd7</t>
+  </si>
+  <si>
+    <t>io_module0</t>
+  </si>
+  <si>
+    <t>io_module0</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>io_module1</t>
+  </si>
+  <si>
+    <t>io_module1</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>io_module2</t>
+  </si>
+  <si>
+    <t>io_module2</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>io_module3</t>
+  </si>
+  <si>
+    <t>io_module3</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>20G</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>24G</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>8G</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd8</t>
+  </si>
+  <si>
+    <t>ssd9</t>
+  </si>
+  <si>
+    <t>ssd10</t>
+  </si>
+  <si>
+    <t>ssd11</t>
+  </si>
+  <si>
+    <t>ssd12</t>
+  </si>
+  <si>
+    <t>ssd13</t>
+  </si>
+  <si>
+    <t>ssd14</t>
+  </si>
+  <si>
+    <t>ssd15</t>
+  </si>
+  <si>
+    <t>ssd16</t>
+  </si>
+  <si>
+    <t>ssd17</t>
+  </si>
+  <si>
+    <t>ssd18</t>
+  </si>
+  <si>
+    <t>ssd19</t>
+  </si>
+  <si>
+    <t>ssd20</t>
+  </si>
+  <si>
+    <t>ssd21</t>
+  </si>
+  <si>
+    <t>ssd22</t>
+  </si>
+  <si>
+    <t>ssd23</t>
+  </si>
+  <si>
+    <t>ssd24</t>
+  </si>
+  <si>
+    <t>ssd25</t>
+  </si>
+  <si>
+    <t>ssd26</t>
+  </si>
+  <si>
+    <t>ssd27</t>
+  </si>
+  <si>
+    <t>ssd28</t>
+  </si>
+  <si>
+    <t>ssd29</t>
+  </si>
+  <si>
+    <t>ssd30</t>
+  </si>
+  <si>
+    <t>ssd31</t>
+  </si>
+  <si>
+    <t>ssd31</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd32</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>ssd33</t>
+  </si>
+  <si>
+    <t>ssd34</t>
+  </si>
+  <si>
+    <t>ssd35</t>
+  </si>
+  <si>
+    <t>ssd36</t>
+  </si>
+  <si>
+    <t>ssd37</t>
+  </si>
+  <si>
+    <t>ssd38</t>
+  </si>
+  <si>
+    <t>ssd39</t>
+  </si>
+  <si>
+    <t>ssd40</t>
+  </si>
+  <si>
+    <t>ssd41</t>
+  </si>
+  <si>
+    <t>ssd42</t>
+  </si>
+  <si>
+    <t>ssd43</t>
+  </si>
+  <si>
+    <t>ssd44</t>
+  </si>
+  <si>
+    <t>ssd45</t>
+  </si>
+  <si>
+    <t>ssd46</t>
+  </si>
+  <si>
+    <t>ssd47</t>
+  </si>
+  <si>
+    <t>ssd48</t>
+  </si>
+  <si>
+    <t>ssd49</t>
+  </si>
+  <si>
+    <t>ssd50</t>
+  </si>
+  <si>
+    <t>ssd51</t>
+  </si>
+  <si>
+    <t>ssd52</t>
+  </si>
+  <si>
+    <t>ssd53</t>
+  </si>
+  <si>
+    <t>ssd54</t>
+  </si>
+  <si>
+    <t>ssd55</t>
+  </si>
+  <si>
+    <t>ssd56</t>
+  </si>
+  <si>
+    <t>ssd57</t>
+  </si>
+  <si>
+    <t>ssd58</t>
+  </si>
+  <si>
+    <t>ssd59</t>
+  </si>
+  <si>
+    <t>ssd60</t>
+  </si>
+  <si>
+    <t>ssd61</t>
+  </si>
+  <si>
+    <t>ssd62</t>
+  </si>
+  <si>
+    <t>ssd63</t>
+  </si>
+  <si>
+    <t>ssd</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>io_module</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>MTBF</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>frontend_module</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>backend_module</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>cpu 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>), Dimm 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, NIC 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개 (가정)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>cpu 16</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Dell </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>자료</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), Dimm 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가정</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>), NIC 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+      </rPr>
+      <t>개 (가정)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>enclosure</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>backplane 1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, fan 4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (2+2), PSU 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>FAN</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <t>PSU</t>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>N (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>전체 개수</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>M (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial Unicode MS"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>최소 개수)</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MTBF </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>배수</t>
+    </r>
+    <phoneticPr fontId="9" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="15">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font/>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="&quot;Malgun Gothic&quot;"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="&quot;Malgun Gothic&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="4">
@@ -249,7 +898,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -265,7 +914,13 @@
     </fill>
   </fills>
   <borders count="7">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -279,27 +934,34 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -309,6 +971,7 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -317,90 +980,86 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="23">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="4" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -590,30 +1249,35 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AN1060"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.63"/>
-    <col customWidth="1" min="2" max="2" width="17.38"/>
-    <col customWidth="1" min="3" max="3" width="18.13"/>
-    <col customWidth="1" min="4" max="5" width="12.63"/>
-    <col customWidth="1" min="6" max="6" width="21.63"/>
-    <col customWidth="1" min="7" max="7" width="18.13"/>
-    <col customWidth="1" min="8" max="8" width="17.5"/>
-    <col customWidth="1" min="9" max="9" width="14.63"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="21.5703125" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1">
+    <row r="1" spans="2:40" ht="15.75" customHeight="1">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -626,627 +1290,1880 @@
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2" ht="15.75" customHeight="1">
-      <c r="B2" s="6" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="22"/>
+    </row>
+    <row r="2" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="X3" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="Z3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="AC3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="AD3" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AE3" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="AL3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="AM3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="AN3" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="I4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J2" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K2" s="7" t="s">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+    </row>
+    <row r="6" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="D6" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="6" t="s">
+      <c r="D7" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B10" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+    </row>
+    <row r="12" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B12" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+    </row>
+    <row r="13" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B13" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+    </row>
+    <row r="14" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+    </row>
+    <row r="16" spans="2:40" ht="15.75" customHeight="1">
+      <c r="B16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B18" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B20" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B21" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B23" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B24" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B26" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B27" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B28" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B30" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B31" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B32" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B33" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B34" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B35" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B36" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B37" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B38" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B39" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B40" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B41" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B42" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B43" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B47" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B49" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B51" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B53" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B55" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="57" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="59" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="60" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="63" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B63" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="64" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B67" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B70" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B71" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1">
+      <c r="A72" s="11"/>
+      <c r="B72" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B73" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B74" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="7" t="s">
+      <c r="C74" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D74" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="7" t="s">
+    </row>
+    <row r="75" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B76" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="D76" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B77" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="D77" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+    </row>
+    <row r="78" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B78" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C78" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="D78" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B79" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C79" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="D79" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="B12" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="H12" s="10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="13" ht="15.75" customHeight="1">
-      <c r="B13" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="H13" s="10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="14" ht="15.75" customHeight="1">
-      <c r="B14" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="H14" s="10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="15" ht="15.75" customHeight="1">
-      <c r="B15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" s="10">
-        <v>1.0</v>
-      </c>
-      <c r="H15" s="10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="16" ht="15.75" customHeight="1">
-      <c r="B16" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="G16" s="10">
-        <v>3.0</v>
-      </c>
-      <c r="H16" s="10">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="17" ht="15.75" customHeight="1">
-      <c r="B17" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" ht="15.75" customHeight="1">
-      <c r="B18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" ht="15.75" customHeight="1">
-      <c r="B19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" ht="15.75" customHeight="1">
-      <c r="B20" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="B21" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1">
-      <c r="B22" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" ht="15.75" customHeight="1">
-      <c r="B23" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" ht="15.75" customHeight="1">
-      <c r="B24" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="25" ht="15.75" customHeight="1">
-      <c r="B25" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="6" t="s">
+    </row>
+    <row r="80" spans="1:8" ht="15.75" customHeight="1">
+      <c r="B80" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="26" ht="15.75" customHeight="1">
-      <c r="B26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="7" t="s">
+      <c r="C80" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B81" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1">
-      <c r="B27" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C27" s="7" t="s">
+      <c r="C81" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D81" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="B28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="30" ht="15.75" customHeight="1">
-      <c r="B30" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="31" ht="15.75" customHeight="1">
-      <c r="B31" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" ht="15.75" customHeight="1">
-      <c r="B32" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" ht="15.75" customHeight="1">
-      <c r="B33" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" ht="15.75" customHeight="1"/>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1"/>
-    <row r="37" ht="15.75" customHeight="1"/>
-    <row r="38" ht="15.75" customHeight="1"/>
-    <row r="39" ht="15.75" customHeight="1"/>
-    <row r="40" ht="15.75" customHeight="1"/>
-    <row r="41" ht="15.75" customHeight="1"/>
-    <row r="42" ht="15.75" customHeight="1"/>
-    <row r="43" ht="15.75" customHeight="1"/>
-    <row r="44" ht="15.75" customHeight="1"/>
-    <row r="45" ht="15.75" customHeight="1"/>
-    <row r="46" ht="15.75" customHeight="1"/>
-    <row r="47" ht="15.75" customHeight="1"/>
-    <row r="48" ht="15.75" customHeight="1"/>
-    <row r="49" ht="15.75" customHeight="1"/>
-    <row r="50" ht="15.75" customHeight="1"/>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
-    <row r="53" ht="15.75" customHeight="1"/>
-    <row r="54" ht="15.75" customHeight="1"/>
-    <row r="55" ht="15.75" customHeight="1"/>
-    <row r="56" ht="15.75" customHeight="1"/>
-    <row r="57" ht="15.75" customHeight="1"/>
-    <row r="58" ht="15.75" customHeight="1"/>
-    <row r="59" ht="15.75" customHeight="1"/>
-    <row r="60" ht="15.75" customHeight="1"/>
-    <row r="61" ht="15.75" customHeight="1"/>
-    <row r="62" ht="15.75" customHeight="1"/>
-    <row r="63" ht="15.75" customHeight="1"/>
-    <row r="64" ht="15.75" customHeight="1"/>
-    <row r="65" ht="15.75" customHeight="1"/>
-    <row r="66" ht="15.75" customHeight="1"/>
-    <row r="67" ht="15.75" customHeight="1"/>
-    <row r="68" ht="15.75" customHeight="1"/>
-    <row r="69" ht="15.75" customHeight="1"/>
-    <row r="70" ht="15.75" customHeight="1"/>
-    <row r="71" ht="15.75" customHeight="1"/>
-    <row r="72" ht="15.75" customHeight="1"/>
-    <row r="73" ht="15.75" customHeight="1"/>
-    <row r="74" ht="15.75" customHeight="1"/>
-    <row r="75" ht="15.75" customHeight="1"/>
-    <row r="76" ht="15.75" customHeight="1"/>
-    <row r="77" ht="15.75" customHeight="1"/>
-    <row r="78" ht="15.75" customHeight="1"/>
-    <row r="79" ht="15.75" customHeight="1"/>
-    <row r="80" ht="15.75" customHeight="1"/>
-    <row r="81" ht="15.75" customHeight="1"/>
-    <row r="82" ht="15.75" customHeight="1"/>
-    <row r="83" ht="15.75" customHeight="1"/>
-    <row r="84" ht="15.75" customHeight="1"/>
-    <row r="85" ht="15.75" customHeight="1"/>
-    <row r="86" ht="15.75" customHeight="1"/>
-    <row r="87" ht="15.75" customHeight="1"/>
-    <row r="88" ht="15.75" customHeight="1"/>
-    <row r="89" ht="15.75" customHeight="1"/>
-    <row r="90" ht="15.75" customHeight="1"/>
-    <row r="91" ht="15.75" customHeight="1"/>
-    <row r="92" ht="15.75" customHeight="1"/>
-    <row r="93" ht="15.75" customHeight="1"/>
-    <row r="94" ht="15.75" customHeight="1"/>
-    <row r="95" ht="15.75" customHeight="1"/>
-    <row r="96" ht="15.75" customHeight="1"/>
-    <row r="97" ht="15.75" customHeight="1"/>
-    <row r="98" ht="15.75" customHeight="1"/>
-    <row r="99" ht="15.75" customHeight="1"/>
-    <row r="100" ht="15.75" customHeight="1"/>
-    <row r="101" ht="15.75" customHeight="1"/>
-    <row r="102" ht="15.75" customHeight="1"/>
-    <row r="103" ht="15.75" customHeight="1"/>
-    <row r="104" ht="15.75" customHeight="1"/>
-    <row r="105" ht="15.75" customHeight="1"/>
-    <row r="106" ht="15.75" customHeight="1"/>
-    <row r="107" ht="15.75" customHeight="1"/>
-    <row r="108" ht="15.75" customHeight="1"/>
-    <row r="109" ht="15.75" customHeight="1"/>
-    <row r="110" ht="15.75" customHeight="1"/>
-    <row r="111" ht="15.75" customHeight="1"/>
-    <row r="112" ht="15.75" customHeight="1"/>
-    <row r="113" ht="15.75" customHeight="1"/>
-    <row r="114" ht="15.75" customHeight="1"/>
-    <row r="115" ht="15.75" customHeight="1"/>
-    <row r="116" ht="15.75" customHeight="1"/>
-    <row r="117" ht="15.75" customHeight="1"/>
-    <row r="118" ht="15.75" customHeight="1"/>
-    <row r="119" ht="15.75" customHeight="1"/>
-    <row r="120" ht="15.75" customHeight="1"/>
-    <row r="121" ht="15.75" customHeight="1"/>
-    <row r="122" ht="15.75" customHeight="1"/>
-    <row r="123" ht="15.75" customHeight="1"/>
-    <row r="124" ht="15.75" customHeight="1"/>
-    <row r="125" ht="15.75" customHeight="1"/>
-    <row r="126" ht="15.75" customHeight="1"/>
-    <row r="127" ht="15.75" customHeight="1"/>
-    <row r="128" ht="15.75" customHeight="1"/>
-    <row r="129" ht="15.75" customHeight="1"/>
-    <row r="130" ht="15.75" customHeight="1"/>
-    <row r="131" ht="15.75" customHeight="1"/>
-    <row r="132" ht="15.75" customHeight="1"/>
-    <row r="133" ht="15.75" customHeight="1"/>
-    <row r="134" ht="15.75" customHeight="1"/>
-    <row r="135" ht="15.75" customHeight="1"/>
-    <row r="136" ht="15.75" customHeight="1"/>
-    <row r="137" ht="15.75" customHeight="1"/>
-    <row r="138" ht="15.75" customHeight="1"/>
-    <row r="139" ht="15.75" customHeight="1"/>
-    <row r="140" ht="15.75" customHeight="1"/>
-    <row r="141" ht="15.75" customHeight="1"/>
-    <row r="142" ht="15.75" customHeight="1"/>
-    <row r="143" ht="15.75" customHeight="1"/>
-    <row r="144" ht="15.75" customHeight="1"/>
-    <row r="145" ht="15.75" customHeight="1"/>
-    <row r="146" ht="15.75" customHeight="1"/>
-    <row r="147" ht="15.75" customHeight="1"/>
-    <row r="148" ht="15.75" customHeight="1"/>
-    <row r="149" ht="15.75" customHeight="1"/>
-    <row r="150" ht="15.75" customHeight="1"/>
-    <row r="151" ht="15.75" customHeight="1"/>
-    <row r="152" ht="15.75" customHeight="1"/>
-    <row r="153" ht="15.75" customHeight="1"/>
-    <row r="154" ht="15.75" customHeight="1"/>
-    <row r="155" ht="15.75" customHeight="1"/>
-    <row r="156" ht="15.75" customHeight="1"/>
-    <row r="157" ht="15.75" customHeight="1"/>
-    <row r="158" ht="15.75" customHeight="1"/>
-    <row r="159" ht="15.75" customHeight="1"/>
-    <row r="160" ht="15.75" customHeight="1"/>
+    </row>
+    <row r="82" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B82" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B83" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B85" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B86" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B87" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B88" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B89" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B90" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B91" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B92" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B93" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B94" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B95" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B96" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B97" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B98" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B99" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B100" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B101" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B103" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B105" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B106" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B107" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B108" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B109" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B110" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B111" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B112" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B113" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B114" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B115" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B116" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B117" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B118" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B119" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B120" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B121" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B122" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B123" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="124" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B124" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="125" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B125" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="126" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B126" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="127" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B127" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D127" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="128" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B128" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D128" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="129" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B129" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="130" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B130" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="131" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B131" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="132" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B132" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D132" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="133" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B133" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="134" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B134" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="135" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B135" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="136" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B136" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="137" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B137" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D137" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="138" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B138" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="139" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B139" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="140" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B140" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="141" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B141" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D141" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="142" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B142" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="D142" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="143" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B143" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="144" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B144" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="145" spans="2:4" ht="15.75" customHeight="1">
+      <c r="B145" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="146" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="147" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="148" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="149" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="150" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="151" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="152" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="153" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="154" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="155" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="156" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="157" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="158" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="159" spans="2:4" ht="15.75" customHeight="1"/>
+    <row r="160" spans="2:4" ht="15.75" customHeight="1"/>
     <row r="161" ht="15.75" customHeight="1"/>
     <row r="162" ht="15.75" customHeight="1"/>
     <row r="163" ht="15.75" customHeight="1"/>
@@ -2091,206 +4008,270 @@
     <row r="1002" ht="15.75" customHeight="1"/>
     <row r="1003" ht="15.75" customHeight="1"/>
     <row r="1004" ht="15.75" customHeight="1"/>
+    <row r="1005" ht="15.75" customHeight="1"/>
+    <row r="1006" ht="15.75" customHeight="1"/>
+    <row r="1007" ht="15.75" customHeight="1"/>
+    <row r="1008" ht="15.75" customHeight="1"/>
+    <row r="1009" ht="15.75" customHeight="1"/>
+    <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
+    <row r="1012" ht="15.75" customHeight="1"/>
+    <row r="1013" ht="15.75" customHeight="1"/>
+    <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
+    <row r="1019" ht="15.75" customHeight="1"/>
+    <row r="1020" ht="15.75" customHeight="1"/>
+    <row r="1021" ht="15.75" customHeight="1"/>
+    <row r="1022" ht="15.75" customHeight="1"/>
+    <row r="1023" ht="15.75" customHeight="1"/>
+    <row r="1024" ht="15.75" customHeight="1"/>
+    <row r="1025" ht="15.75" customHeight="1"/>
+    <row r="1026" ht="15.75" customHeight="1"/>
+    <row r="1027" ht="15.75" customHeight="1"/>
+    <row r="1028" ht="15.75" customHeight="1"/>
+    <row r="1029" ht="15.75" customHeight="1"/>
+    <row r="1030" ht="15.75" customHeight="1"/>
+    <row r="1031" ht="15.75" customHeight="1"/>
+    <row r="1032" ht="15.75" customHeight="1"/>
+    <row r="1033" ht="15.75" customHeight="1"/>
+    <row r="1034" ht="15.75" customHeight="1"/>
+    <row r="1035" ht="15.75" customHeight="1"/>
+    <row r="1036" ht="15.75" customHeight="1"/>
+    <row r="1037" ht="15.75" customHeight="1"/>
+    <row r="1038" ht="15.75" customHeight="1"/>
+    <row r="1039" ht="15.75" customHeight="1"/>
+    <row r="1040" ht="15.75" customHeight="1"/>
+    <row r="1041" ht="15.75" customHeight="1"/>
+    <row r="1042" ht="15.75" customHeight="1"/>
+    <row r="1043" ht="15.75" customHeight="1"/>
+    <row r="1044" ht="15.75" customHeight="1"/>
+    <row r="1045" ht="15.75" customHeight="1"/>
+    <row r="1046" ht="15.75" customHeight="1"/>
+    <row r="1047" ht="15.75" customHeight="1"/>
+    <row r="1048" ht="15.75" customHeight="1"/>
+    <row r="1049" ht="15.75" customHeight="1"/>
+    <row r="1050" ht="15.75" customHeight="1"/>
+    <row r="1051" ht="15.75" customHeight="1"/>
+    <row r="1052" ht="15.75" customHeight="1"/>
+    <row r="1053" ht="15.75" customHeight="1"/>
+    <row r="1054" ht="15.75" customHeight="1"/>
+    <row r="1055" ht="15.75" customHeight="1"/>
+    <row r="1056" ht="15.75" customHeight="1"/>
+    <row r="1057" ht="15.75" customHeight="1"/>
+    <row r="1058" ht="15.75" customHeight="1"/>
+    <row r="1059" ht="15.75" customHeight="1"/>
+    <row r="1060" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:L1"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B1:G1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="12.63"/>
-    <col customWidth="1" min="2" max="2" width="15.88"/>
-    <col customWidth="1" min="3" max="4" width="12.63"/>
-    <col customWidth="1" min="5" max="5" width="18.13"/>
-    <col customWidth="1" min="6" max="6" width="12.63"/>
-    <col customWidth="1" min="7" max="7" width="16.0"/>
-    <col customWidth="1" min="8" max="8" width="12.63"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="4" width="12.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1"/>
-    <row r="2" ht="15.75" customHeight="1">
+    <row r="1" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="2" spans="2:7" ht="15.75" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>29</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C3" s="11">
-        <v>2000000.0</v>
-      </c>
-      <c r="D3" s="11">
-        <v>8.0</v>
-      </c>
-      <c r="E3" s="9">
-        <f t="shared" ref="E3:E7" si="1"> C3 / (C3+D3)</f>
-        <v>0.999996</v>
-      </c>
-      <c r="F3" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" s="14">
-        <v>4194389.0</v>
-      </c>
-      <c r="D4" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="E4" s="9">
-        <f t="shared" si="1"/>
-        <v>0.9999980927</v>
-      </c>
-      <c r="F4" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="14">
-        <v>4194389.0</v>
-      </c>
-      <c r="D5" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="E5" s="9">
-        <f t="shared" si="1"/>
-        <v>0.9999980927</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C6" s="11">
-        <v>1500000.0</v>
-      </c>
-      <c r="D6" s="11">
-        <v>8.0</v>
-      </c>
-      <c r="E6" s="9">
-        <f t="shared" si="1"/>
-        <v>0.9999946667</v>
-      </c>
-      <c r="F6" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="14">
-        <v>2500000.0</v>
-      </c>
-      <c r="D7" s="14">
-        <v>8.0</v>
-      </c>
-      <c r="E7" s="9">
-        <f t="shared" si="1"/>
-        <v>0.9999968</v>
-      </c>
-      <c r="F7" s="11">
-        <v>3.0</v>
-      </c>
-      <c r="G7" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="11">
-        <v>0.9999994</v>
-      </c>
-      <c r="F8" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="11">
-        <v>0.9999994</v>
-      </c>
-      <c r="F9" s="11">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="11">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1"/>
-    <row r="11" ht="15.75" customHeight="1"/>
-    <row r="12" ht="15.75" customHeight="1"/>
-    <row r="13" ht="15.75" customHeight="1"/>
-    <row r="14" ht="15.75" customHeight="1"/>
-    <row r="15" ht="15.75" customHeight="1"/>
-    <row r="16" ht="15.75" customHeight="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="17">
+        <v>233360</v>
+      </c>
+      <c r="D3" s="4">
+        <v>72</v>
+      </c>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E7" si="0">C3 / (C3+D3)</f>
+        <v>0.9996915589979094</v>
+      </c>
+      <c r="F3" s="4">
+        <v>1</v>
+      </c>
+      <c r="G3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="18">
+        <f>newSheet!F6</f>
+        <v>696379.86455637566</v>
+      </c>
+      <c r="D4" s="6">
+        <v>72</v>
+      </c>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9998966188423577</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="18">
+        <f>newSheet!F7</f>
+        <v>713363.52244140836</v>
+      </c>
+      <c r="D5" s="6">
+        <v>72</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99989907987794946</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1</v>
+      </c>
+      <c r="G5" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B6" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="4">
+        <v>4194389</v>
+      </c>
+      <c r="D6" s="4">
+        <v>72</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>0.9999828345048386</v>
+      </c>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B7" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="6">
+        <v>2500000</v>
+      </c>
+      <c r="D7" s="6">
+        <v>8</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.99999680001023994</v>
+      </c>
+      <c r="F7" s="4">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="19">
+        <f>newSheet!F8</f>
+        <v>380992.90066414548</v>
+      </c>
+      <c r="D8" s="4">
+        <v>72</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.99999939999999998</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="19">
+        <f>newSheet!F8</f>
+        <v>380992.90066414548</v>
+      </c>
+      <c r="D9" s="4">
+        <v>72</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.99999939999999998</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1</v>
+      </c>
+      <c r="G9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="11" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="12" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="13" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="14" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="15" spans="2:7" ht="15.75" customHeight="1"/>
+    <row r="16" spans="2:7" ht="15.75" customHeight="1"/>
     <row r="17" ht="15.75" customHeight="1"/>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -3277,109 +5258,190 @@
     <row r="1000" ht="15.75" customHeight="1"/>
     <row r="1001" ht="15.75" customHeight="1"/>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A4:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="40.28515625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="4">
-      <c r="A4" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="18">
-        <v>367985.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="18">
-        <v>3.51E8</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B7" s="18">
-        <v>3472222.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="18">
-        <v>4194389.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="B9" s="18">
-        <v>2500000.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="B10" s="18">
-        <v>9247903.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="18">
-        <v>1.3764075E7</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B12" s="18">
-        <v>1500000.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="18">
-        <v>8249472.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="B14" s="18">
-        <v>241296.0</v>
+    <row r="4" spans="1:11" ht="14.25">
+      <c r="A4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15" customHeight="1">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="10">
+        <v>367985</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="10">
+        <v>351000000</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6" s="15">
+        <f>1 /( 1/B6 * 16 + 1 / B7 * 4 + 1/B8)</f>
+        <v>696379.86455637566</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="10">
+        <v>3472222</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="F7" s="15">
+        <f>1 /( 1/B6 * 4 + 1 / B7 * 4 + 1/B8)</f>
+        <v>713363.52244140836</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <f>(I7-J7+1)/J7</f>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" s="10">
+        <v>4194389</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8" s="16">
+        <f>1/(1/B10 + 1/B12/K7 + 1/B14/K8)</f>
+        <v>380992.90066414548</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="I8">
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f>(I8-J8+1)/J8</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="14.25">
+      <c r="A9" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="10">
+        <v>2500000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="14.25">
+      <c r="A10" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="10">
+        <v>9247903</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="14.25">
+      <c r="A11" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="10">
+        <v>13764075</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="14.25">
+      <c r="A12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="10">
+        <v>1500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="14.25">
+      <c r="A13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="10">
+        <v>8249472</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="14.25">
+      <c r="A14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="10">
+        <v>241296</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>